<commit_message>
Codigo Teoria de Muestras Grandes
</commit_message>
<xml_diff>
--- a/Finanzas/1_Ene-Abr_2018.xlsx
+++ b/Finanzas/1_Ene-Abr_2018.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="341">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -1032,6 +1032,21 @@
   </si>
   <si>
     <t>Clases 2 y 3</t>
+  </si>
+  <si>
+    <t>Café Ale</t>
+  </si>
+  <si>
+    <t>Ale Trabajo</t>
+  </si>
+  <si>
+    <t>Cihina</t>
+  </si>
+  <si>
+    <t>Depósito</t>
+  </si>
+  <si>
+    <t>Mamá Depósito</t>
   </si>
 </sst>
 </file>
@@ -1400,7 +1415,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1609,6 +1624,7 @@
     <xf numFmtId="0" fontId="13" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1905,8 +1921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="V41" sqref="V41"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1983,7 +1999,7 @@
       <c r="E2" s="56"/>
       <c r="F2" s="114">
         <f>N3-D2</f>
-        <v>4865</v>
+        <v>5865</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>2</v>
@@ -2110,7 +2126,7 @@
       </c>
       <c r="N3" s="25">
         <f>(SUM(D2,(K11:K499)))-(SUM((J11:J499),(I11:I499)))</f>
-        <v>5763</v>
+        <v>6763</v>
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
@@ -2186,7 +2202,7 @@
       </c>
       <c r="P4" s="79">
         <f>SUM(N3,R9,P7)</f>
-        <v>40131</v>
+        <v>41761</v>
       </c>
       <c r="Z4" s="47">
         <v>43108</v>
@@ -2365,7 +2381,7 @@
       </c>
       <c r="N6" s="52">
         <f>(SUM((W11:W299),(AC3:AC500),(I11:I499)))-(SUM((X11:X499)))</f>
-        <v>1548</v>
+        <v>1178</v>
       </c>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
@@ -2453,12 +2469,12 @@
       </c>
       <c r="P7" s="78">
         <f>SUM(R7,N6)</f>
-        <v>548</v>
+        <v>1178</v>
       </c>
       <c r="Q7" s="75"/>
       <c r="R7" s="74">
         <f>(SUM(X11:X499))-(SUM(K11:K499))</f>
-        <v>-1000</v>
+        <v>0</v>
       </c>
       <c r="S7" s="116"/>
       <c r="T7" s="118">
@@ -4233,11 +4249,17 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G24" s="99"/>
-      <c r="H24" s="56"/>
+      <c r="G24" s="99">
+        <v>43209</v>
+      </c>
+      <c r="H24" s="56" t="s">
+        <v>13</v>
+      </c>
       <c r="I24" s="101"/>
       <c r="J24" s="102"/>
-      <c r="K24" s="103"/>
+      <c r="K24" s="103">
+        <v>1000</v>
+      </c>
       <c r="M24" s="59">
         <v>42802</v>
       </c>
@@ -5895,7 +5917,9 @@
         <v>106</v>
       </c>
       <c r="V41" s="35"/>
-      <c r="W41" s="37"/>
+      <c r="W41" s="37">
+        <v>150</v>
+      </c>
       <c r="X41" s="37"/>
       <c r="Z41" s="47">
         <v>43145</v>
@@ -5984,7 +6008,9 @@
         <v>317</v>
       </c>
       <c r="V42" s="35"/>
-      <c r="W42" s="37"/>
+      <c r="W42" s="37">
+        <v>500</v>
+      </c>
       <c r="X42" s="37"/>
       <c r="Z42" s="47">
         <v>43146</v>
@@ -6070,11 +6096,13 @@
         <v>43209</v>
       </c>
       <c r="U43" s="35" t="s">
-        <v>24</v>
+        <v>339</v>
       </c>
       <c r="V43" s="35"/>
       <c r="W43" s="37"/>
-      <c r="X43" s="37"/>
+      <c r="X43" s="37">
+        <v>1000</v>
+      </c>
       <c r="Z43" s="47">
         <v>43147</v>
       </c>
@@ -6158,10 +6186,16 @@
         <v>0</v>
       </c>
       <c r="T44" s="36"/>
-      <c r="U44" s="35"/>
+      <c r="U44" s="35" t="s">
+        <v>340</v>
+      </c>
       <c r="V44" s="35"/>
-      <c r="W44" s="37"/>
-      <c r="X44" s="87"/>
+      <c r="W44" s="37">
+        <v>1000</v>
+      </c>
+      <c r="X44" s="124">
+        <v>1000</v>
+      </c>
       <c r="Z44" s="47">
         <v>43148</v>
       </c>
@@ -11155,7 +11189,7 @@
       </c>
       <c r="AC102" s="41">
         <f t="shared" si="12"/>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="AD102" s="107">
         <v>120</v>
@@ -11164,7 +11198,7 @@
       <c r="AF102" s="56"/>
       <c r="AG102" s="51">
         <f t="shared" si="10"/>
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="AH102" s="56">
         <v>70</v>
@@ -11173,7 +11207,9 @@
         <v>155</v>
       </c>
       <c r="AJ102" s="56"/>
-      <c r="AK102" s="56"/>
+      <c r="AK102" s="56">
+        <v>10</v>
+      </c>
       <c r="AL102" s="56"/>
       <c r="AM102" s="56"/>
       <c r="AN102" s="56"/>
@@ -11246,7 +11282,7 @@
       </c>
       <c r="AC103" s="41">
         <f t="shared" si="12"/>
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="AD103" s="107">
         <v>80</v>
@@ -11255,10 +11291,14 @@
       <c r="AF103" s="56"/>
       <c r="AG103" s="51">
         <f t="shared" si="10"/>
-        <v>28</v>
-      </c>
-      <c r="AH103" s="56"/>
-      <c r="AI103" s="56"/>
+        <v>78</v>
+      </c>
+      <c r="AH103" s="56">
+        <v>50</v>
+      </c>
+      <c r="AI103" s="56" t="s">
+        <v>338</v>
+      </c>
       <c r="AJ103" s="56"/>
       <c r="AK103" s="56"/>
       <c r="AL103" s="56"/>
@@ -11326,22 +11366,32 @@
       <c r="AA104" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="AB104" s="49"/>
+      <c r="AB104" s="49" t="s">
+        <v>314</v>
+      </c>
       <c r="AC104" s="41">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD104" s="107"/>
+        <v>20</v>
+      </c>
+      <c r="AD104" s="107">
+        <v>80</v>
+      </c>
       <c r="AE104" s="107"/>
       <c r="AF104" s="56"/>
       <c r="AG104" s="51">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AH104" s="56"/>
-      <c r="AI104" s="56"/>
+        <v>60</v>
+      </c>
+      <c r="AH104" s="56">
+        <v>50</v>
+      </c>
+      <c r="AI104" s="56" t="s">
+        <v>114</v>
+      </c>
       <c r="AJ104" s="56"/>
-      <c r="AK104" s="56"/>
+      <c r="AK104" s="56">
+        <v>10</v>
+      </c>
       <c r="AL104" s="56"/>
       <c r="AM104" s="56"/>
       <c r="AN104" s="56"/>
@@ -11403,22 +11453,34 @@
       <c r="AA105" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="AB105" s="49"/>
+      <c r="AB105" s="49" t="s">
+        <v>337</v>
+      </c>
       <c r="AC105" s="41">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD105" s="107"/>
+        <v>-60</v>
+      </c>
+      <c r="AD105" s="107">
+        <v>80</v>
+      </c>
       <c r="AE105" s="107"/>
       <c r="AF105" s="56"/>
       <c r="AG105" s="51">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AH105" s="56"/>
-      <c r="AI105" s="56"/>
-      <c r="AJ105" s="56"/>
-      <c r="AK105" s="56"/>
+        <v>140</v>
+      </c>
+      <c r="AH105" s="56">
+        <v>70</v>
+      </c>
+      <c r="AI105" s="56" t="s">
+        <v>191</v>
+      </c>
+      <c r="AJ105" s="56" t="s">
+        <v>336</v>
+      </c>
+      <c r="AK105" s="56">
+        <v>70</v>
+      </c>
       <c r="AL105" s="56"/>
       <c r="AM105" s="56"/>
       <c r="AN105" s="56"/>
@@ -11483,9 +11545,11 @@
       <c r="AB106" s="49"/>
       <c r="AC106" s="41">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD106" s="107"/>
+        <v>80</v>
+      </c>
+      <c r="AD106" s="107">
+        <v>80</v>
+      </c>
       <c r="AE106" s="107"/>
       <c r="AF106" s="56"/>
       <c r="AG106" s="51">

</xml_diff>

<commit_message>
MOM MLE y LSRE
</commit_message>
<xml_diff>
--- a/Finanzas/1_Ene-Abr_2018.xlsx
+++ b/Finanzas/1_Ene-Abr_2018.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Finanzas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="343">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -1047,6 +1042,12 @@
   </si>
   <si>
     <t>Mamá Depósito</t>
+  </si>
+  <si>
+    <t>Starbucks</t>
+  </si>
+  <si>
+    <t>Taxi1, Taxi2, Taxi3, Taxi 4</t>
   </si>
 </sst>
 </file>
@@ -1911,7 +1912,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1921,8 +1922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2202,7 +2203,7 @@
       </c>
       <c r="P4" s="79">
         <f>SUM(N3,R9,P7)</f>
-        <v>41761</v>
+        <v>41786</v>
       </c>
       <c r="Z4" s="47">
         <v>43108</v>
@@ -2275,7 +2276,7 @@
       </c>
       <c r="BG4" s="57">
         <f>(SUM((AV3:AV519)))-(SUM((AZ3:AZ519)))</f>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="BH4" s="57"/>
     </row>
@@ -2381,7 +2382,7 @@
       </c>
       <c r="N6" s="52">
         <f>(SUM((W11:W299),(AC3:AC500),(I11:I499)))-(SUM((X11:X499)))</f>
-        <v>1178</v>
+        <v>1203</v>
       </c>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
@@ -2469,7 +2470,7 @@
       </c>
       <c r="P7" s="78">
         <f>SUM(R7,N6)</f>
-        <v>1178</v>
+        <v>1203</v>
       </c>
       <c r="Q7" s="75"/>
       <c r="R7" s="74">
@@ -12009,22 +12010,40 @@
       <c r="AB112" s="49"/>
       <c r="AC112" s="41">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD112" s="107"/>
-      <c r="AE112" s="107"/>
+        <v>25</v>
+      </c>
+      <c r="AD112" s="107">
+        <v>250</v>
+      </c>
+      <c r="AE112" s="107">
+        <v>200</v>
+      </c>
       <c r="AF112" s="56"/>
       <c r="AG112" s="51">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AH112" s="56"/>
-      <c r="AI112" s="56"/>
-      <c r="AJ112" s="56"/>
-      <c r="AK112" s="56"/>
-      <c r="AL112" s="56"/>
-      <c r="AM112" s="56"/>
-      <c r="AN112" s="56"/>
+        <v>425</v>
+      </c>
+      <c r="AH112" s="56">
+        <v>200</v>
+      </c>
+      <c r="AI112" s="56" t="s">
+        <v>341</v>
+      </c>
+      <c r="AJ112" s="56" t="s">
+        <v>342</v>
+      </c>
+      <c r="AK112" s="56">
+        <v>55</v>
+      </c>
+      <c r="AL112" s="56">
+        <v>50</v>
+      </c>
+      <c r="AM112" s="56">
+        <v>45</v>
+      </c>
+      <c r="AN112" s="56">
+        <v>50</v>
+      </c>
       <c r="AO112" s="56"/>
       <c r="AP112" s="56"/>
       <c r="AQ112" s="56"/>
@@ -12033,22 +12052,28 @@
       <c r="AT112" s="56"/>
       <c r="AU112">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AV112" s="56"/>
+        <v>25</v>
+      </c>
+      <c r="AV112" s="56">
+        <v>20</v>
+      </c>
       <c r="AW112" s="56"/>
       <c r="AX112" s="56"/>
-      <c r="AY112" s="56"/>
+      <c r="AY112" s="56">
+        <v>2</v>
+      </c>
       <c r="AZ112" s="56">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BA112" s="56"/>
       <c r="BB112">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="BC112" s="56"/>
+      <c r="BC112" s="56">
+        <v>5</v>
+      </c>
       <c r="BD112" s="56"/>
       <c r="BE112" s="56"/>
       <c r="BF112" s="56"/>

</xml_diff>